<commit_message>
feat: update PST pie chart color
</commit_message>
<xml_diff>
--- a/templates/finance/Personal Spending Tracker (PST).xlsx
+++ b/templates/finance/Personal Spending Tracker (PST).xlsx
@@ -160,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,8 +169,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9900"/>
-        <bgColor rgb="FFFF9900"/>
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -324,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -333,13 +345,13 @@
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -347,7 +359,7 @@
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -357,8 +369,8 @@
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="4" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="15" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
@@ -372,11 +384,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="16" fillId="3" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="16" fillId="5" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -399,7 +414,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4472C4"/>
+                <a:srgbClr val="27AE60"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -447,7 +462,7 @@
               <a:solidFill>
                 <a:srgbClr val="1A1A1A"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
         </a:p>
@@ -491,7 +506,8 @@
     </c:title>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
+      <c:barChart>
+        <c:barDir val="col"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -501,15 +517,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
-                <a:srgbClr val="4472C4"/>
+                <a:srgbClr val="000000"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Dashboard!$F$26:$F$37</c:f>
@@ -521,8 +537,11 @@
               <c:numCache/>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
+        <c:axId val="1024569598"/>
+        <c:axId val="1786107236"/>
+      </c:barChart>
+      <c:lineChart>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -709,11 +728,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1894180203"/>
-        <c:axId val="1763590054"/>
+        <c:axId val="1024569598"/>
+        <c:axId val="1786107236"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1894180203"/>
+        <c:axId val="1024569598"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -765,10 +784,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1763590054"/>
+        <c:crossAx val="1786107236"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1763590054"/>
+        <c:axId val="1786107236"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -838,12 +857,12 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1894180203"/>
+        <c:crossAx val="1024569598"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -858,7 +877,7 @@
               <a:solidFill>
                 <a:srgbClr val="1A1A1A"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
         </a:p>
@@ -903,7 +922,7 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7419975" cy="4476750"/>
+    <xdr:ext cx="7658100" cy="4476750"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="776178337" name="Chart 2" title="Chart"/>
@@ -1142,7 +1161,9 @@
     <col customWidth="1" min="8" max="8" width="11.44"/>
     <col customWidth="1" min="9" max="9" width="14.44"/>
     <col customWidth="1" min="10" max="10" width="14.0"/>
-    <col customWidth="1" min="11" max="25" width="10.56"/>
+    <col customWidth="1" min="11" max="11" width="10.56"/>
+    <col customWidth="1" min="12" max="12" width="13.0"/>
+    <col customWidth="1" min="13" max="25" width="10.56"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1"/>
@@ -1267,15 +1288,15 @@
       </c>
       <c r="G27" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!G$25, Spending!$E$2:$E1003, Dashboard!$F27)</f>
-        <v>1900000</v>
+        <v>700000</v>
       </c>
       <c r="H27" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!H$25, Spending!$E$2:$E1003, Dashboard!$F27)</f>
-        <v>250000</v>
+        <v>100000</v>
       </c>
       <c r="I27" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!I$25, Spending!$E$2:$E1003, Dashboard!$F27)</f>
-        <v>915000</v>
+        <v>1100000</v>
       </c>
       <c r="J27" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!J$25, Spending!$E$2:$E1003, Dashboard!$F27)</f>
@@ -1283,11 +1304,11 @@
       </c>
       <c r="K27" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!K$25, Spending!$E$2:$E1003, Dashboard!$F27)</f>
-        <v>100000</v>
+        <v>150000</v>
       </c>
       <c r="L27" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!L$25, Spending!$E$2:$E1003, Dashboard!$F27)</f>
-        <v>250000</v>
+        <v>1365000</v>
       </c>
       <c r="M27" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!M$25, Spending!$E$2:$E1003, Dashboard!$F27)</f>
@@ -1305,15 +1326,15 @@
       </c>
       <c r="G28" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!G$25, Spending!$E$2:$E1003, Dashboard!$F28)</f>
-        <v>1900000</v>
+        <v>1100000</v>
       </c>
       <c r="H28" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!H$25, Spending!$E$2:$E1003, Dashboard!$F28)</f>
-        <v>250000</v>
+        <v>365000</v>
       </c>
       <c r="I28" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!I$25, Spending!$E$2:$E1003, Dashboard!$F28)</f>
-        <v>915000</v>
+        <v>1600000</v>
       </c>
       <c r="J28" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!J$25, Spending!$E$2:$E1003, Dashboard!$F28)</f>
@@ -1343,27 +1364,27 @@
       </c>
       <c r="G29" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!G$25, Spending!$E$2:$E1003, Dashboard!$F29)</f>
-        <v>1900000</v>
+        <v>400000</v>
       </c>
       <c r="H29" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!H$25, Spending!$E$2:$E1003, Dashboard!$F29)</f>
-        <v>250000</v>
+        <v>100000</v>
       </c>
       <c r="I29" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!I$25, Spending!$E$2:$E1003, Dashboard!$F29)</f>
-        <v>915000</v>
+        <v>1100000</v>
       </c>
       <c r="J29" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!J$25, Spending!$E$2:$E1003, Dashboard!$F29)</f>
-        <v>100000</v>
+        <v>365000</v>
       </c>
       <c r="K29" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!K$25, Spending!$E$2:$E1003, Dashboard!$F29)</f>
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="L29" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!L$25, Spending!$E$2:$E1003, Dashboard!$F29)</f>
-        <v>250000</v>
+        <v>550000</v>
       </c>
       <c r="M29" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!M$25, Spending!$E$2:$E1003, Dashboard!$F29)</f>
@@ -1381,15 +1402,15 @@
       </c>
       <c r="G30" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!G$25, Spending!$E$2:$E1003, Dashboard!$F30)</f>
-        <v>1900000</v>
+        <v>700000</v>
       </c>
       <c r="H30" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!H$25, Spending!$E$2:$E1003, Dashboard!$F30)</f>
-        <v>250000</v>
+        <v>1000000</v>
       </c>
       <c r="I30" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!I$25, Spending!$E$2:$E1003, Dashboard!$F30)</f>
-        <v>915000</v>
+        <v>1415000</v>
       </c>
       <c r="J30" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!J$25, Spending!$E$2:$E1003, Dashboard!$F30)</f>
@@ -1401,7 +1422,7 @@
       </c>
       <c r="L30" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!L$25, Spending!$E$2:$E1003, Dashboard!$F30)</f>
-        <v>250000</v>
+        <v>200000</v>
       </c>
       <c r="M30" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!M$25, Spending!$E$2:$E1003, Dashboard!$F30)</f>
@@ -1419,15 +1440,15 @@
       </c>
       <c r="G31" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!G$25, Spending!$E$2:$E1003, Dashboard!$F31)</f>
-        <v>1900000</v>
+        <v>250000</v>
       </c>
       <c r="H31" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!H$25, Spending!$E$2:$E1003, Dashboard!$F31)</f>
-        <v>250000</v>
+        <v>900000</v>
       </c>
       <c r="I31" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!I$25, Spending!$E$2:$E1003, Dashboard!$F31)</f>
-        <v>915000</v>
+        <v>1350000</v>
       </c>
       <c r="J31" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!J$25, Spending!$E$2:$E1003, Dashboard!$F31)</f>
@@ -1435,11 +1456,11 @@
       </c>
       <c r="K31" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!K$25, Spending!$E$2:$E1003, Dashboard!$F31)</f>
-        <v>100000</v>
+        <v>365000</v>
       </c>
       <c r="L31" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!L$25, Spending!$E$2:$E1003, Dashboard!$F31)</f>
-        <v>250000</v>
+        <v>550000</v>
       </c>
       <c r="M31" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!M$25, Spending!$E$2:$E1003, Dashboard!$F31)</f>
@@ -1457,19 +1478,19 @@
       </c>
       <c r="G32" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!G$25, Spending!$E$2:$E1003, Dashboard!$F32)</f>
-        <v>1900000</v>
+        <v>1265000</v>
       </c>
       <c r="H32" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!H$25, Spending!$E$2:$E1003, Dashboard!$F32)</f>
-        <v>250000</v>
+        <v>100000</v>
       </c>
       <c r="I32" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!I$25, Spending!$E$2:$E1003, Dashboard!$F32)</f>
-        <v>915000</v>
+        <v>800000</v>
       </c>
       <c r="J32" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!J$25, Spending!$E$2:$E1003, Dashboard!$F32)</f>
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="K32" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!K$25, Spending!$E$2:$E1003, Dashboard!$F32)</f>
@@ -1495,15 +1516,15 @@
       </c>
       <c r="G33" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!G$25, Spending!$E$2:$E1003, Dashboard!$F33)</f>
-        <v>1900000</v>
+        <v>1050000</v>
       </c>
       <c r="H33" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!H$25, Spending!$E$2:$E1003, Dashboard!$F33)</f>
-        <v>250000</v>
+        <v>100000</v>
       </c>
       <c r="I33" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!I$25, Spending!$E$2:$E1003, Dashboard!$F33)</f>
-        <v>915000</v>
+        <v>1615000</v>
       </c>
       <c r="J33" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!J$25, Spending!$E$2:$E1003, Dashboard!$F33)</f>
@@ -1511,11 +1532,11 @@
       </c>
       <c r="K33" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!K$25, Spending!$E$2:$E1003, Dashboard!$F33)</f>
-        <v>100000</v>
+        <v>450000</v>
       </c>
       <c r="L33" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!L$25, Spending!$E$2:$E1003, Dashboard!$F33)</f>
-        <v>250000</v>
+        <v>200000</v>
       </c>
       <c r="M33" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!M$25, Spending!$E$2:$E1003, Dashboard!$F33)</f>
@@ -1533,19 +1554,19 @@
       </c>
       <c r="G34" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!G$25, Spending!$E$2:$E1003, Dashboard!$F34)</f>
-        <v>1900000</v>
+        <v>615000</v>
       </c>
       <c r="H34" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!H$25, Spending!$E$2:$E1003, Dashboard!$F34)</f>
-        <v>250000</v>
+        <v>100000</v>
       </c>
       <c r="I34" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!I$25, Spending!$E$2:$E1003, Dashboard!$F34)</f>
-        <v>915000</v>
+        <v>700000</v>
       </c>
       <c r="J34" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!J$25, Spending!$E$2:$E1003, Dashboard!$F34)</f>
-        <v>100000</v>
+        <v>900000</v>
       </c>
       <c r="K34" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!K$25, Spending!$E$2:$E1003, Dashboard!$F34)</f>
@@ -1553,7 +1574,7 @@
       </c>
       <c r="L34" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!L$25, Spending!$E$2:$E1003, Dashboard!$F34)</f>
-        <v>250000</v>
+        <v>1100000</v>
       </c>
       <c r="M34" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!M$25, Spending!$E$2:$E1003, Dashboard!$F34)</f>
@@ -1571,27 +1592,27 @@
       </c>
       <c r="G35" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!G$25, Spending!$E$2:$E1003, Dashboard!$F35)</f>
-        <v>1900000</v>
+        <v>350000</v>
       </c>
       <c r="H35" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!H$25, Spending!$E$2:$E1003, Dashboard!$F35)</f>
-        <v>250000</v>
+        <v>900000</v>
       </c>
       <c r="I35" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!I$25, Spending!$E$2:$E1003, Dashboard!$F35)</f>
-        <v>915000</v>
+        <v>565000</v>
       </c>
       <c r="J35" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!J$25, Spending!$E$2:$E1003, Dashboard!$F35)</f>
-        <v>100000</v>
+        <v>150000</v>
       </c>
       <c r="K35" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!K$25, Spending!$E$2:$E1003, Dashboard!$F35)</f>
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="L35" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!L$25, Spending!$E$2:$E1003, Dashboard!$F35)</f>
-        <v>250000</v>
+        <v>550000</v>
       </c>
       <c r="M35" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!M$25, Spending!$E$2:$E1003, Dashboard!$F35)</f>
@@ -1609,15 +1630,15 @@
       </c>
       <c r="G36" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!G$25, Spending!$E$2:$E1003, Dashboard!$F36)</f>
-        <v>1900000</v>
+        <v>600000</v>
       </c>
       <c r="H36" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!H$25, Spending!$E$2:$E1003, Dashboard!$F36)</f>
-        <v>250000</v>
+        <v>100000</v>
       </c>
       <c r="I36" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!I$25, Spending!$E$2:$E1003, Dashboard!$F36)</f>
-        <v>915000</v>
+        <v>1200000</v>
       </c>
       <c r="J36" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!J$25, Spending!$E$2:$E1003, Dashboard!$F36)</f>
@@ -1625,11 +1646,11 @@
       </c>
       <c r="K36" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!K$25, Spending!$E$2:$E1003, Dashboard!$F36)</f>
-        <v>100000</v>
+        <v>900000</v>
       </c>
       <c r="L36" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!L$25, Spending!$E$2:$E1003, Dashboard!$F36)</f>
-        <v>250000</v>
+        <v>615000</v>
       </c>
       <c r="M36" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!M$25, Spending!$E$2:$E1003, Dashboard!$F36)</f>
@@ -1649,15 +1670,15 @@
       </c>
       <c r="G37" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!G$25, Spending!$E$2:$E1003, Dashboard!$F37)</f>
-        <v>1900000</v>
+        <v>615000</v>
       </c>
       <c r="H37" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!H$25, Spending!$E$2:$E1003, Dashboard!$F37)</f>
-        <v>250000</v>
+        <v>1000000</v>
       </c>
       <c r="I37" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!I$25, Spending!$E$2:$E1003, Dashboard!$F37)</f>
-        <v>915000</v>
+        <v>1500000</v>
       </c>
       <c r="J37" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!J$25, Spending!$E$2:$E1003, Dashboard!$F37)</f>
@@ -1669,7 +1690,7 @@
       </c>
       <c r="L37" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!L$25, Spending!$E$2:$E1003, Dashboard!$F37)</f>
-        <v>250000</v>
+        <v>200000</v>
       </c>
       <c r="M37" s="15">
         <f>SUMIFS(Spending!$F$2:$F1003, Spending!$C$2:$C1003, Dashboard!M$25, Spending!$E$2:$E1003, Dashboard!$F37)</f>
@@ -1679,27 +1700,27 @@
     <row r="38" ht="15.75" customHeight="1">
       <c r="G38" s="19">
         <f t="shared" ref="G38:M38" si="1">SUM(G26:G37)</f>
-        <v>22800000</v>
+        <v>9545000</v>
       </c>
       <c r="H38" s="19">
         <f t="shared" si="1"/>
-        <v>3000000</v>
+        <v>5015000</v>
       </c>
       <c r="I38" s="19">
         <f t="shared" si="1"/>
-        <v>10980000</v>
+        <v>13860000</v>
       </c>
       <c r="J38" s="19">
         <f t="shared" si="1"/>
-        <v>1200000</v>
+        <v>3215000</v>
       </c>
       <c r="K38" s="19">
         <f t="shared" si="1"/>
-        <v>1200000</v>
+        <v>4465000</v>
       </c>
       <c r="L38" s="19">
         <f t="shared" si="1"/>
-        <v>3000000</v>
+        <v>6080000</v>
       </c>
       <c r="M38" s="19">
         <f t="shared" si="1"/>
@@ -2688,7 +2709,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <tabColor rgb="FFFF9900"/>
+    <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
@@ -2965,8 +2986,8 @@
         <f t="shared" ref="E13:E22" si="2">TEXT(D13,"MMMM")</f>
         <v>February</v>
       </c>
-      <c r="F13" s="26">
-        <v>100000.0</v>
+      <c r="F13" s="30">
+        <v>150000.0</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
@@ -2986,7 +3007,7 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -3007,8 +3028,8 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F15" s="26">
-        <v>450000.0</v>
+      <c r="F15" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
@@ -3028,8 +3049,8 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F16" s="26">
-        <v>365000.0</v>
+      <c r="F16" s="30">
+        <v>900000.0</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
@@ -3049,7 +3070,7 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -3070,8 +3091,8 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F18" s="26">
-        <v>1000000.0</v>
+      <c r="F18" s="30">
+        <v>250000.0</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
@@ -3091,8 +3112,8 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F19" s="26">
-        <v>250000.0</v>
+      <c r="F19" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
@@ -3112,8 +3133,8 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F20" s="26">
-        <v>900000.0</v>
+      <c r="F20" s="30">
+        <v>450000.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -3133,8 +3154,8 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F21" s="26">
-        <v>150000.0</v>
+      <c r="F21" s="30">
+        <v>365000.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -3154,8 +3175,8 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F22" s="26">
-        <v>100000.0</v>
+      <c r="F22" s="30">
+        <v>1000000.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -3186,7 +3207,7 @@
         <f t="shared" ref="E24:E33" si="3">TEXT(D24,"MMMM")</f>
         <v>March</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -3207,8 +3228,8 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F25" s="26">
-        <v>100000.0</v>
+      <c r="F25" s="30">
+        <v>250000.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -3228,8 +3249,8 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F26" s="26">
-        <v>450000.0</v>
+      <c r="F26" s="30">
+        <v>900000.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -3249,8 +3270,8 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F27" s="26">
-        <v>365000.0</v>
+      <c r="F27" s="30">
+        <v>450000.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -3270,7 +3291,7 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F28" s="26">
+      <c r="F28" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -3291,8 +3312,8 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F29" s="26">
-        <v>1000000.0</v>
+      <c r="F29" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -3312,8 +3333,8 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F30" s="26">
-        <v>250000.0</v>
+      <c r="F30" s="30">
+        <v>365000.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -3333,8 +3354,8 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F31" s="26">
-        <v>900000.0</v>
+      <c r="F31" s="30">
+        <v>1000000.0</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -3354,8 +3375,8 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F32" s="26">
-        <v>150000.0</v>
+      <c r="F32" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
@@ -3375,8 +3396,8 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F33" s="26">
-        <v>100000.0</v>
+      <c r="F33" s="30">
+        <v>150000.0</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -3407,8 +3428,8 @@
         <f t="shared" ref="E35:E44" si="4">TEXT(D35,"MMMM")</f>
         <v>April</v>
       </c>
-      <c r="F35" s="26">
-        <v>100000.0</v>
+      <c r="F35" s="30">
+        <v>1000000.0</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
@@ -3428,8 +3449,8 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F36" s="26">
-        <v>100000.0</v>
+      <c r="F36" s="30">
+        <v>900000.0</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
@@ -3449,8 +3470,8 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F37" s="26">
-        <v>450000.0</v>
+      <c r="F37" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
@@ -3470,8 +3491,8 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F38" s="26">
-        <v>365000.0</v>
+      <c r="F38" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
@@ -3491,8 +3512,8 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F39" s="26">
-        <v>100000.0</v>
+      <c r="F39" s="30">
+        <v>365000.0</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
@@ -3512,8 +3533,8 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F40" s="26">
-        <v>1000000.0</v>
+      <c r="F40" s="30">
+        <v>150000.0</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
@@ -3533,8 +3554,8 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F41" s="26">
-        <v>250000.0</v>
+      <c r="F41" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
@@ -3554,8 +3575,8 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F42" s="26">
-        <v>900000.0</v>
+      <c r="F42" s="30">
+        <v>250000.0</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
@@ -3575,8 +3596,8 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F43" s="26">
-        <v>150000.0</v>
+      <c r="F43" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -3596,8 +3617,8 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F44" s="26">
-        <v>100000.0</v>
+      <c r="F44" s="30">
+        <v>450000.0</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
@@ -3628,7 +3649,7 @@
         <f t="shared" ref="E46:E55" si="5">TEXT(D46,"MMMM")</f>
         <v>May</v>
       </c>
-      <c r="F46" s="26">
+      <c r="F46" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -3649,8 +3670,8 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F47" s="26">
-        <v>100000.0</v>
+      <c r="F47" s="30">
+        <v>900000.0</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
@@ -3670,8 +3691,8 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F48" s="26">
-        <v>450000.0</v>
+      <c r="F48" s="30">
+        <v>365000.0</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
@@ -3691,8 +3712,8 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F49" s="26">
-        <v>365000.0</v>
+      <c r="F49" s="30">
+        <v>150000.0</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
@@ -3712,7 +3733,7 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F50" s="26">
+      <c r="F50" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -3733,8 +3754,8 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F51" s="26">
-        <v>1000000.0</v>
+      <c r="F51" s="30">
+        <v>450000.0</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
@@ -3754,8 +3775,8 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F52" s="26">
-        <v>250000.0</v>
+      <c r="F52" s="30">
+        <v>1000000.0</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
@@ -3775,8 +3796,8 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F53" s="26">
-        <v>900000.0</v>
+      <c r="F53" s="30">
+        <v>250000.0</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
@@ -3796,8 +3817,8 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F54" s="26">
-        <v>150000.0</v>
+      <c r="F54" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
@@ -3817,7 +3838,7 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F55" s="26">
+      <c r="F55" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -3849,8 +3870,8 @@
         <f t="shared" ref="E57:E66" si="6">TEXT(D57,"MMMM")</f>
         <v>June</v>
       </c>
-      <c r="F57" s="26">
-        <v>100000.0</v>
+      <c r="F57" s="30">
+        <v>365000.0</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
@@ -3870,8 +3891,8 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F58" s="26">
-        <v>100000.0</v>
+      <c r="F58" s="30">
+        <v>1000000.0</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
@@ -3891,8 +3912,8 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F59" s="26">
-        <v>450000.0</v>
+      <c r="F59" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
@@ -3912,8 +3933,8 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F60" s="26">
-        <v>365000.0</v>
+      <c r="F60" s="30">
+        <v>250000.0</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
@@ -3933,7 +3954,7 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F61" s="26">
+      <c r="F61" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -3954,8 +3975,8 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F62" s="26">
-        <v>1000000.0</v>
+      <c r="F62" s="30">
+        <v>150000.0</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
@@ -3975,8 +3996,8 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F63" s="26">
-        <v>250000.0</v>
+      <c r="F63" s="30">
+        <v>900000.0</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
@@ -3996,8 +4017,8 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F64" s="26">
-        <v>900000.0</v>
+      <c r="F64" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
@@ -4017,8 +4038,8 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F65" s="26">
-        <v>150000.0</v>
+      <c r="F65" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
@@ -4038,8 +4059,8 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F66" s="26">
-        <v>100000.0</v>
+      <c r="F66" s="30">
+        <v>450000.0</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
@@ -4070,7 +4091,7 @@
         <f t="shared" ref="E68:E77" si="7">TEXT(D68,"MMMM")</f>
         <v>July</v>
       </c>
-      <c r="F68" s="26">
+      <c r="F68" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -4091,7 +4112,7 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F69" s="26">
+      <c r="F69" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -4112,7 +4133,7 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F70" s="26">
+      <c r="F70" s="30">
         <v>450000.0</v>
       </c>
     </row>
@@ -4133,8 +4154,8 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F71" s="26">
-        <v>365000.0</v>
+      <c r="F71" s="30">
+        <v>250000.0</v>
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
@@ -4154,8 +4175,8 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F72" s="26">
-        <v>100000.0</v>
+      <c r="F72" s="30">
+        <v>1000000.0</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
@@ -4175,8 +4196,8 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F73" s="26">
-        <v>1000000.0</v>
+      <c r="F73" s="30">
+        <v>900000.0</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
@@ -4196,8 +4217,8 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F74" s="26">
-        <v>250000.0</v>
+      <c r="F74" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
@@ -4217,8 +4238,8 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F75" s="26">
-        <v>900000.0</v>
+      <c r="F75" s="30">
+        <v>365000.0</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
@@ -4238,7 +4259,7 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F76" s="26">
+      <c r="F76" s="30">
         <v>150000.0</v>
       </c>
     </row>
@@ -4259,7 +4280,7 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F77" s="26">
+      <c r="F77" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -4291,8 +4312,8 @@
         <f t="shared" ref="E79:E88" si="8">TEXT(D79,"MMMM")</f>
         <v>August</v>
       </c>
-      <c r="F79" s="26">
-        <v>100000.0</v>
+      <c r="F79" s="30">
+        <v>450000.0</v>
       </c>
     </row>
     <row r="80" ht="15.75" customHeight="1">
@@ -4312,8 +4333,8 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F80" s="26">
-        <v>100000.0</v>
+      <c r="F80" s="30">
+        <v>1000000.0</v>
       </c>
     </row>
     <row r="81" ht="15.75" customHeight="1">
@@ -4333,8 +4354,8 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F81" s="26">
-        <v>450000.0</v>
+      <c r="F81" s="30">
+        <v>250000.0</v>
       </c>
     </row>
     <row r="82" ht="15.75" customHeight="1">
@@ -4354,7 +4375,7 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F82" s="26">
+      <c r="F82" s="30">
         <v>365000.0</v>
       </c>
     </row>
@@ -4375,7 +4396,7 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F83" s="26">
+      <c r="F83" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -4396,8 +4417,8 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F84" s="26">
-        <v>1000000.0</v>
+      <c r="F84" s="30">
+        <v>150000.0</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
@@ -4417,8 +4438,8 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F85" s="26">
-        <v>250000.0</v>
+      <c r="F85" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
@@ -4438,7 +4459,7 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F86" s="26">
+      <c r="F86" s="30">
         <v>900000.0</v>
       </c>
     </row>
@@ -4459,8 +4480,8 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F87" s="26">
-        <v>150000.0</v>
+      <c r="F87" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="88" ht="15.75" customHeight="1">
@@ -4480,7 +4501,7 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F88" s="26">
+      <c r="F88" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -4512,7 +4533,7 @@
         <f t="shared" ref="E90:E99" si="9">TEXT(D90,"MMMM")</f>
         <v>September</v>
       </c>
-      <c r="F90" s="26">
+      <c r="F90" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -4533,8 +4554,8 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F91" s="26">
-        <v>100000.0</v>
+      <c r="F91" s="30">
+        <v>450000.0</v>
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
@@ -4554,8 +4575,8 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F92" s="26">
-        <v>450000.0</v>
+      <c r="F92" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
@@ -4575,8 +4596,8 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F93" s="26">
-        <v>365000.0</v>
+      <c r="F93" s="30">
+        <v>150000.0</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
@@ -4596,8 +4617,8 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F94" s="26">
-        <v>100000.0</v>
+      <c r="F94" s="30">
+        <v>900000.0</v>
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1">
@@ -4617,8 +4638,8 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F95" s="26">
-        <v>1000000.0</v>
+      <c r="F95" s="30">
+        <v>250000.0</v>
       </c>
     </row>
     <row r="96" ht="15.75" customHeight="1">
@@ -4638,8 +4659,8 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F96" s="26">
-        <v>250000.0</v>
+      <c r="F96" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="97" ht="15.75" customHeight="1">
@@ -4659,8 +4680,8 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F97" s="26">
-        <v>900000.0</v>
+      <c r="F97" s="30">
+        <v>365000.0</v>
       </c>
     </row>
     <row r="98" ht="15.75" customHeight="1">
@@ -4680,8 +4701,8 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F98" s="26">
-        <v>150000.0</v>
+      <c r="F98" s="30">
+        <v>1000000.0</v>
       </c>
     </row>
     <row r="99" ht="15.75" customHeight="1">
@@ -4701,7 +4722,7 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F99" s="26">
+      <c r="F99" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -4733,8 +4754,8 @@
         <f t="shared" ref="E101:E110" si="10">TEXT(D101,"MMMM")</f>
         <v>October</v>
       </c>
-      <c r="F101" s="26">
-        <v>100000.0</v>
+      <c r="F101" s="30">
+        <v>1000000.0</v>
       </c>
     </row>
     <row r="102" ht="15.75" customHeight="1">
@@ -4754,7 +4775,7 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F102" s="26">
+      <c r="F102" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -4775,8 +4796,8 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F103" s="26">
-        <v>450000.0</v>
+      <c r="F103" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
@@ -4796,7 +4817,7 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F104" s="26">
+      <c r="F104" s="30">
         <v>365000.0</v>
       </c>
     </row>
@@ -4817,8 +4838,8 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F105" s="26">
-        <v>100000.0</v>
+      <c r="F105" s="30">
+        <v>150000.0</v>
       </c>
     </row>
     <row r="106" ht="15.75" customHeight="1">
@@ -4838,8 +4859,8 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F106" s="26">
-        <v>1000000.0</v>
+      <c r="F106" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="107" ht="15.75" customHeight="1">
@@ -4859,8 +4880,8 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F107" s="26">
-        <v>250000.0</v>
+      <c r="F107" s="30">
+        <v>900000.0</v>
       </c>
     </row>
     <row r="108" ht="15.75" customHeight="1">
@@ -4880,8 +4901,8 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F108" s="26">
-        <v>900000.0</v>
+      <c r="F108" s="30">
+        <v>250000.0</v>
       </c>
     </row>
     <row r="109" ht="15.75" customHeight="1">
@@ -4901,8 +4922,8 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F109" s="26">
-        <v>150000.0</v>
+      <c r="F109" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="110" ht="15.75" customHeight="1">
@@ -4922,8 +4943,8 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F110" s="26">
-        <v>100000.0</v>
+      <c r="F110" s="30">
+        <v>450000.0</v>
       </c>
     </row>
     <row r="111" ht="15.75" customHeight="1">
@@ -4954,8 +4975,8 @@
         <f t="shared" ref="E112:E121" si="11">TEXT(D112,"MMMM")</f>
         <v>November</v>
       </c>
-      <c r="F112" s="26">
-        <v>100000.0</v>
+      <c r="F112" s="30">
+        <v>900000.0</v>
       </c>
     </row>
     <row r="113" ht="15.75" customHeight="1">
@@ -4975,8 +4996,8 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F113" s="26">
-        <v>100000.0</v>
+      <c r="F113" s="30">
+        <v>1000000.0</v>
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1">
@@ -4996,8 +5017,8 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F114" s="26">
-        <v>450000.0</v>
+      <c r="F114" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1">
@@ -5017,8 +5038,8 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F115" s="26">
-        <v>365000.0</v>
+      <c r="F115" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1">
@@ -5038,7 +5059,7 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F116" s="26">
+      <c r="F116" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -5059,8 +5080,8 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F117" s="26">
-        <v>1000000.0</v>
+      <c r="F117" s="30">
+        <v>450000.0</v>
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
@@ -5080,8 +5101,8 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F118" s="26">
-        <v>250000.0</v>
+      <c r="F118" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
@@ -5101,8 +5122,8 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F119" s="26">
-        <v>900000.0</v>
+      <c r="F119" s="30">
+        <v>150000.0</v>
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1">
@@ -5122,8 +5143,8 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F120" s="26">
-        <v>150000.0</v>
+      <c r="F120" s="30">
+        <v>365000.0</v>
       </c>
     </row>
     <row r="121" ht="15.75" customHeight="1">
@@ -5143,8 +5164,8 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F121" s="26">
-        <v>100000.0</v>
+      <c r="F121" s="30">
+        <v>250000.0</v>
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1">
@@ -5175,7 +5196,7 @@
         <f t="shared" ref="E123:E132" si="12">TEXT(D123,"MMMM")</f>
         <v>December</v>
       </c>
-      <c r="F123" s="26">
+      <c r="F123" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -5196,8 +5217,8 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F124" s="26">
-        <v>100000.0</v>
+      <c r="F124" s="30">
+        <v>900000.0</v>
       </c>
     </row>
     <row r="125" ht="15.75" customHeight="1">
@@ -5217,8 +5238,8 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F125" s="26">
-        <v>450000.0</v>
+      <c r="F125" s="30">
+        <v>150000.0</v>
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1">
@@ -5238,8 +5259,8 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F126" s="26">
-        <v>365000.0</v>
+      <c r="F126" s="30">
+        <v>450000.0</v>
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
@@ -5259,7 +5280,7 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F127" s="26">
+      <c r="F127" s="30">
         <v>100000.0</v>
       </c>
     </row>
@@ -5280,8 +5301,8 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F128" s="26">
-        <v>1000000.0</v>
+      <c r="F128" s="30">
+        <v>365000.0</v>
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
@@ -5301,8 +5322,8 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F129" s="26">
-        <v>250000.0</v>
+      <c r="F129" s="30">
+        <v>1000000.0</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
@@ -5322,8 +5343,8 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F130" s="26">
-        <v>900000.0</v>
+      <c r="F130" s="30">
+        <v>250000.0</v>
       </c>
     </row>
     <row r="131" ht="15.75" customHeight="1">
@@ -5343,8 +5364,8 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F131" s="26">
-        <v>150000.0</v>
+      <c r="F131" s="30">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="132" ht="15.75" customHeight="1">
@@ -5364,7 +5385,7 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F132" s="26">
+      <c r="F132" s="30">
         <v>100000.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: Monthly Spending heading to small
</commit_message>
<xml_diff>
--- a/templates/finance/Personal Spending Tracker (PST).xlsx
+++ b/templates/finance/Personal Spending Tracker (PST).xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="35">
   <si>
     <t>Monthly Spending</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Month</t>
   </si>
   <si>
-    <t>Type</t>
+    <t>Category</t>
   </si>
   <si>
     <t>Groceries</t>
@@ -91,9 +91,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -121,10 +118,10 @@
     <t>Coffee</t>
   </si>
   <si>
-    <t>Entertainment (XXI)</t>
+    <t>Subscriptions (Netflix)</t>
   </si>
   <si>
-    <t>Subscriptions (Netflix)</t>
+    <t>Entertainment (XXI)</t>
   </si>
 </sst>
 </file>
@@ -135,7 +132,7 @@
     <numFmt numFmtId="164" formatCode="[$Rp-421]#,##0"/>
     <numFmt numFmtId="165" formatCode="D/M/YYYY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -144,11 +141,17 @@
     </font>
     <font>
       <b/>
+      <sz val="24.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font/>
+    <font>
+      <b/>
       <sz val="12.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -336,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -345,51 +348,54 @@
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
+    <xf borderId="5" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="4" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="15" fillId="4" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="15" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="3" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="15" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="15" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="16" fillId="5" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="16" fillId="5" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -506,8 +512,7 @@
     </c:title>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
+      <c:lineChart>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -517,15 +522,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
-                <a:srgbClr val="000000"/>
+                <a:srgbClr val="4472C4"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Dashboard!$F$26:$F$37</c:f>
@@ -537,11 +542,8 @@
               <c:numCache/>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1024569598"/>
-        <c:axId val="1786107236"/>
-      </c:barChart>
-      <c:lineChart>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -728,11 +730,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1024569598"/>
-        <c:axId val="1786107236"/>
+        <c:axId val="368659382"/>
+        <c:axId val="127607972"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1024569598"/>
+        <c:axId val="368659382"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -784,10 +786,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1786107236"/>
+        <c:crossAx val="127607972"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1786107236"/>
+        <c:axId val="127607972"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -862,7 +864,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1024569598"/>
+        <c:crossAx val="368659382"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2694,10 +2696,10 @@
     <row r="1003" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="G24:M24"/>
+    <mergeCell ref="A24:D37"/>
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="F24:F25"/>
-    <mergeCell ref="A24:D37"/>
+    <mergeCell ref="G24:M24"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -2736,16 +2738,16 @@
         <v>23</v>
       </c>
       <c r="C1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>24</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>25</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -2753,7 +2755,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>8</v>
@@ -2774,7 +2776,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>6</v>
@@ -2795,7 +2797,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>6</v>
@@ -2816,7 +2818,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>6</v>
@@ -2837,7 +2839,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="23" t="s">
         <v>7</v>
@@ -2879,7 +2881,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="23" t="s">
         <v>5</v>
@@ -2900,7 +2902,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>4</v>
@@ -2920,8 +2922,8 @@
       <c r="A10" s="22">
         <v>9.0</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>34</v>
+      <c r="B10" s="27" t="s">
+        <v>9</v>
       </c>
       <c r="C10" s="23" t="s">
         <v>9</v>
@@ -2942,7 +2944,7 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" s="23" t="s">
         <v>9</v>
@@ -2959,22 +2961,22 @@
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="27" t="str">
+      <c r="A12" s="28" t="str">
         <f>E11</f>
         <v>January</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="22">
         <v>1.0</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>8</v>
@@ -2986,7 +2988,7 @@
         <f t="shared" ref="E13:E22" si="2">TEXT(D13,"MMMM")</f>
         <v>February</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="31">
         <v>150000.0</v>
       </c>
     </row>
@@ -2995,7 +2997,7 @@
         <v>2.0</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="23" t="s">
         <v>6</v>
@@ -3007,7 +3009,7 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3016,7 +3018,7 @@
         <v>3.0</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="23" t="s">
         <v>6</v>
@@ -3028,7 +3030,7 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3037,7 +3039,7 @@
         <v>4.0</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="23" t="s">
         <v>6</v>
@@ -3049,7 +3051,7 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="31">
         <v>900000.0</v>
       </c>
     </row>
@@ -3058,7 +3060,7 @@
         <v>5.0</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>7</v>
@@ -3070,7 +3072,7 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F17" s="30">
+      <c r="F17" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3091,7 +3093,7 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="31">
         <v>250000.0</v>
       </c>
     </row>
@@ -3100,7 +3102,7 @@
         <v>7.0</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="23" t="s">
         <v>5</v>
@@ -3112,7 +3114,7 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3121,7 +3123,7 @@
         <v>8.0</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>4</v>
@@ -3133,7 +3135,7 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F20" s="31">
         <v>450000.0</v>
       </c>
     </row>
@@ -3154,7 +3156,7 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F21" s="31">
         <v>365000.0</v>
       </c>
     </row>
@@ -3163,7 +3165,7 @@
         <v>10.0</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C22" s="23" t="s">
         <v>9</v>
@@ -3175,27 +3177,27 @@
         <f t="shared" si="2"/>
         <v>February</v>
       </c>
-      <c r="F22" s="30">
+      <c r="F22" s="31">
         <v>1000000.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="27" t="str">
+      <c r="A23" s="28" t="str">
         <f>E22</f>
         <v>February</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="30"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="22">
         <v>1.0</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="23" t="s">
         <v>8</v>
@@ -3207,7 +3209,7 @@
         <f t="shared" ref="E24:E33" si="3">TEXT(D24,"MMMM")</f>
         <v>March</v>
       </c>
-      <c r="F24" s="30">
+      <c r="F24" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3216,7 +3218,7 @@
         <v>2.0</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="23" t="s">
         <v>6</v>
@@ -3228,7 +3230,7 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F25" s="30">
+      <c r="F25" s="31">
         <v>250000.0</v>
       </c>
     </row>
@@ -3237,7 +3239,7 @@
         <v>3.0</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="23" t="s">
         <v>6</v>
@@ -3249,7 +3251,7 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F26" s="30">
+      <c r="F26" s="31">
         <v>900000.0</v>
       </c>
     </row>
@@ -3258,7 +3260,7 @@
         <v>4.0</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" s="23" t="s">
         <v>6</v>
@@ -3270,7 +3272,7 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F27" s="30">
+      <c r="F27" s="31">
         <v>450000.0</v>
       </c>
     </row>
@@ -3279,7 +3281,7 @@
         <v>5.0</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="23" t="s">
         <v>7</v>
@@ -3291,7 +3293,7 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F28" s="30">
+      <c r="F28" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3312,7 +3314,7 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F29" s="30">
+      <c r="F29" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3321,7 +3323,7 @@
         <v>7.0</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="23" t="s">
         <v>5</v>
@@ -3333,7 +3335,7 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F30" s="30">
+      <c r="F30" s="31">
         <v>365000.0</v>
       </c>
     </row>
@@ -3342,7 +3344,7 @@
         <v>8.0</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="23" t="s">
         <v>4</v>
@@ -3354,7 +3356,7 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F31" s="30">
+      <c r="F31" s="31">
         <v>1000000.0</v>
       </c>
     </row>
@@ -3375,7 +3377,7 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F32" s="30">
+      <c r="F32" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3384,7 +3386,7 @@
         <v>10.0</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C33" s="23" t="s">
         <v>9</v>
@@ -3396,27 +3398,27 @@
         <f t="shared" si="3"/>
         <v>March</v>
       </c>
-      <c r="F33" s="30">
+      <c r="F33" s="31">
         <v>150000.0</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="27" t="str">
+      <c r="A34" s="28" t="str">
         <f>E33</f>
         <v>March</v>
       </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="29"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="30"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="22">
         <v>1.0</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C35" s="23" t="s">
         <v>8</v>
@@ -3428,7 +3430,7 @@
         <f t="shared" ref="E35:E44" si="4">TEXT(D35,"MMMM")</f>
         <v>April</v>
       </c>
-      <c r="F35" s="30">
+      <c r="F35" s="31">
         <v>1000000.0</v>
       </c>
     </row>
@@ -3437,7 +3439,7 @@
         <v>2.0</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C36" s="23" t="s">
         <v>6</v>
@@ -3449,7 +3451,7 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F36" s="30">
+      <c r="F36" s="31">
         <v>900000.0</v>
       </c>
     </row>
@@ -3458,7 +3460,7 @@
         <v>3.0</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" s="23" t="s">
         <v>6</v>
@@ -3470,7 +3472,7 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F37" s="30">
+      <c r="F37" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3479,7 +3481,7 @@
         <v>4.0</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38" s="23" t="s">
         <v>6</v>
@@ -3491,7 +3493,7 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F38" s="30">
+      <c r="F38" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3500,7 +3502,7 @@
         <v>5.0</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="23" t="s">
         <v>7</v>
@@ -3512,7 +3514,7 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F39" s="30">
+      <c r="F39" s="31">
         <v>365000.0</v>
       </c>
     </row>
@@ -3533,7 +3535,7 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F40" s="30">
+      <c r="F40" s="31">
         <v>150000.0</v>
       </c>
     </row>
@@ -3542,7 +3544,7 @@
         <v>7.0</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C41" s="23" t="s">
         <v>5</v>
@@ -3554,7 +3556,7 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F41" s="30">
+      <c r="F41" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3563,7 +3565,7 @@
         <v>8.0</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C42" s="23" t="s">
         <v>4</v>
@@ -3575,7 +3577,7 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F42" s="30">
+      <c r="F42" s="31">
         <v>250000.0</v>
       </c>
     </row>
@@ -3596,7 +3598,7 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F43" s="30">
+      <c r="F43" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3605,7 +3607,7 @@
         <v>10.0</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C44" s="23" t="s">
         <v>9</v>
@@ -3617,27 +3619,27 @@
         <f t="shared" si="4"/>
         <v>April</v>
       </c>
-      <c r="F44" s="30">
+      <c r="F44" s="31">
         <v>450000.0</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="27" t="str">
+      <c r="A45" s="28" t="str">
         <f>E44</f>
         <v>April</v>
       </c>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="29"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="30"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="22">
         <v>1.0</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C46" s="23" t="s">
         <v>8</v>
@@ -3649,7 +3651,7 @@
         <f t="shared" ref="E46:E55" si="5">TEXT(D46,"MMMM")</f>
         <v>May</v>
       </c>
-      <c r="F46" s="30">
+      <c r="F46" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3658,7 +3660,7 @@
         <v>2.0</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C47" s="23" t="s">
         <v>6</v>
@@ -3670,7 +3672,7 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F47" s="30">
+      <c r="F47" s="31">
         <v>900000.0</v>
       </c>
     </row>
@@ -3679,7 +3681,7 @@
         <v>3.0</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C48" s="23" t="s">
         <v>6</v>
@@ -3691,7 +3693,7 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F48" s="30">
+      <c r="F48" s="31">
         <v>365000.0</v>
       </c>
     </row>
@@ -3700,7 +3702,7 @@
         <v>4.0</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C49" s="23" t="s">
         <v>6</v>
@@ -3712,7 +3714,7 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F49" s="30">
+      <c r="F49" s="31">
         <v>150000.0</v>
       </c>
     </row>
@@ -3721,7 +3723,7 @@
         <v>5.0</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C50" s="23" t="s">
         <v>7</v>
@@ -3733,7 +3735,7 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F50" s="30">
+      <c r="F50" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3754,7 +3756,7 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F51" s="30">
+      <c r="F51" s="31">
         <v>450000.0</v>
       </c>
     </row>
@@ -3763,7 +3765,7 @@
         <v>7.0</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C52" s="23" t="s">
         <v>5</v>
@@ -3775,7 +3777,7 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F52" s="30">
+      <c r="F52" s="31">
         <v>1000000.0</v>
       </c>
     </row>
@@ -3784,7 +3786,7 @@
         <v>8.0</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C53" s="23" t="s">
         <v>4</v>
@@ -3796,7 +3798,7 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F53" s="30">
+      <c r="F53" s="31">
         <v>250000.0</v>
       </c>
     </row>
@@ -3817,7 +3819,7 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F54" s="30">
+      <c r="F54" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3826,7 +3828,7 @@
         <v>10.0</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C55" s="23" t="s">
         <v>9</v>
@@ -3838,27 +3840,27 @@
         <f t="shared" si="5"/>
         <v>May</v>
       </c>
-      <c r="F55" s="30">
+      <c r="F55" s="31">
         <v>100000.0</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="27" t="str">
+      <c r="A56" s="28" t="str">
         <f>E55</f>
         <v>May</v>
       </c>
-      <c r="B56" s="28"/>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="29"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="30"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="22">
         <v>1.0</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C57" s="23" t="s">
         <v>8</v>
@@ -3870,7 +3872,7 @@
         <f t="shared" ref="E57:E66" si="6">TEXT(D57,"MMMM")</f>
         <v>June</v>
       </c>
-      <c r="F57" s="30">
+      <c r="F57" s="31">
         <v>365000.0</v>
       </c>
     </row>
@@ -3879,7 +3881,7 @@
         <v>2.0</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C58" s="23" t="s">
         <v>6</v>
@@ -3891,7 +3893,7 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F58" s="30">
+      <c r="F58" s="31">
         <v>1000000.0</v>
       </c>
     </row>
@@ -3900,7 +3902,7 @@
         <v>3.0</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C59" s="23" t="s">
         <v>6</v>
@@ -3912,7 +3914,7 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F59" s="30">
+      <c r="F59" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3921,7 +3923,7 @@
         <v>4.0</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C60" s="23" t="s">
         <v>6</v>
@@ -3933,7 +3935,7 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F60" s="30">
+      <c r="F60" s="31">
         <v>250000.0</v>
       </c>
     </row>
@@ -3942,7 +3944,7 @@
         <v>5.0</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C61" s="23" t="s">
         <v>7</v>
@@ -3954,7 +3956,7 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F61" s="30">
+      <c r="F61" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -3975,7 +3977,7 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F62" s="30">
+      <c r="F62" s="31">
         <v>150000.0</v>
       </c>
     </row>
@@ -3984,7 +3986,7 @@
         <v>7.0</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C63" s="23" t="s">
         <v>5</v>
@@ -3996,7 +3998,7 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F63" s="30">
+      <c r="F63" s="31">
         <v>900000.0</v>
       </c>
     </row>
@@ -4005,7 +4007,7 @@
         <v>8.0</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C64" s="23" t="s">
         <v>4</v>
@@ -4017,7 +4019,7 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F64" s="30">
+      <c r="F64" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -4038,7 +4040,7 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F65" s="30">
+      <c r="F65" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -4047,7 +4049,7 @@
         <v>10.0</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C66" s="23" t="s">
         <v>9</v>
@@ -4059,27 +4061,27 @@
         <f t="shared" si="6"/>
         <v>June</v>
       </c>
-      <c r="F66" s="30">
+      <c r="F66" s="31">
         <v>450000.0</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="27" t="str">
+      <c r="A67" s="28" t="str">
         <f>E66</f>
         <v>June</v>
       </c>
-      <c r="B67" s="28"/>
-      <c r="C67" s="28"/>
-      <c r="D67" s="28"/>
-      <c r="E67" s="28"/>
-      <c r="F67" s="29"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="30"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="22">
         <v>1.0</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C68" s="23" t="s">
         <v>8</v>
@@ -4091,7 +4093,7 @@
         <f t="shared" ref="E68:E77" si="7">TEXT(D68,"MMMM")</f>
         <v>July</v>
       </c>
-      <c r="F68" s="30">
+      <c r="F68" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -4100,7 +4102,7 @@
         <v>2.0</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C69" s="23" t="s">
         <v>6</v>
@@ -4112,7 +4114,7 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F69" s="30">
+      <c r="F69" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -4121,7 +4123,7 @@
         <v>3.0</v>
       </c>
       <c r="B70" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C70" s="23" t="s">
         <v>6</v>
@@ -4133,7 +4135,7 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F70" s="30">
+      <c r="F70" s="31">
         <v>450000.0</v>
       </c>
     </row>
@@ -4142,7 +4144,7 @@
         <v>4.0</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C71" s="23" t="s">
         <v>6</v>
@@ -4154,7 +4156,7 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F71" s="30">
+      <c r="F71" s="31">
         <v>250000.0</v>
       </c>
     </row>
@@ -4163,7 +4165,7 @@
         <v>5.0</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C72" s="23" t="s">
         <v>7</v>
@@ -4175,7 +4177,7 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F72" s="30">
+      <c r="F72" s="31">
         <v>1000000.0</v>
       </c>
     </row>
@@ -4196,7 +4198,7 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F73" s="30">
+      <c r="F73" s="31">
         <v>900000.0</v>
       </c>
     </row>
@@ -4205,7 +4207,7 @@
         <v>7.0</v>
       </c>
       <c r="B74" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C74" s="23" t="s">
         <v>5</v>
@@ -4217,7 +4219,7 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F74" s="30">
+      <c r="F74" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -4226,7 +4228,7 @@
         <v>8.0</v>
       </c>
       <c r="B75" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C75" s="23" t="s">
         <v>4</v>
@@ -4238,7 +4240,7 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F75" s="30">
+      <c r="F75" s="31">
         <v>365000.0</v>
       </c>
     </row>
@@ -4259,7 +4261,7 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F76" s="30">
+      <c r="F76" s="31">
         <v>150000.0</v>
       </c>
     </row>
@@ -4268,7 +4270,7 @@
         <v>10.0</v>
       </c>
       <c r="B77" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C77" s="23" t="s">
         <v>9</v>
@@ -4280,27 +4282,27 @@
         <f t="shared" si="7"/>
         <v>July</v>
       </c>
-      <c r="F77" s="30">
+      <c r="F77" s="31">
         <v>100000.0</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="27" t="str">
+      <c r="A78" s="28" t="str">
         <f>E77</f>
         <v>July</v>
       </c>
-      <c r="B78" s="28"/>
-      <c r="C78" s="28"/>
-      <c r="D78" s="28"/>
-      <c r="E78" s="28"/>
-      <c r="F78" s="29"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="30"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="22">
         <v>1.0</v>
       </c>
       <c r="B79" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C79" s="23" t="s">
         <v>8</v>
@@ -4312,7 +4314,7 @@
         <f t="shared" ref="E79:E88" si="8">TEXT(D79,"MMMM")</f>
         <v>August</v>
       </c>
-      <c r="F79" s="30">
+      <c r="F79" s="31">
         <v>450000.0</v>
       </c>
     </row>
@@ -4321,7 +4323,7 @@
         <v>2.0</v>
       </c>
       <c r="B80" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C80" s="23" t="s">
         <v>6</v>
@@ -4333,7 +4335,7 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F80" s="30">
+      <c r="F80" s="31">
         <v>1000000.0</v>
       </c>
     </row>
@@ -4342,7 +4344,7 @@
         <v>3.0</v>
       </c>
       <c r="B81" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C81" s="23" t="s">
         <v>6</v>
@@ -4354,7 +4356,7 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F81" s="30">
+      <c r="F81" s="31">
         <v>250000.0</v>
       </c>
     </row>
@@ -4363,7 +4365,7 @@
         <v>4.0</v>
       </c>
       <c r="B82" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C82" s="23" t="s">
         <v>6</v>
@@ -4375,7 +4377,7 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F82" s="30">
+      <c r="F82" s="31">
         <v>365000.0</v>
       </c>
     </row>
@@ -4384,7 +4386,7 @@
         <v>5.0</v>
       </c>
       <c r="B83" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C83" s="23" t="s">
         <v>7</v>
@@ -4396,7 +4398,7 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F83" s="30">
+      <c r="F83" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -4417,7 +4419,7 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F84" s="30">
+      <c r="F84" s="31">
         <v>150000.0</v>
       </c>
     </row>
@@ -4426,7 +4428,7 @@
         <v>7.0</v>
       </c>
       <c r="B85" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C85" s="23" t="s">
         <v>5</v>
@@ -4438,7 +4440,7 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F85" s="30">
+      <c r="F85" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -4447,7 +4449,7 @@
         <v>8.0</v>
       </c>
       <c r="B86" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C86" s="23" t="s">
         <v>4</v>
@@ -4459,7 +4461,7 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F86" s="30">
+      <c r="F86" s="31">
         <v>900000.0</v>
       </c>
     </row>
@@ -4480,7 +4482,7 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F87" s="30">
+      <c r="F87" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -4489,7 +4491,7 @@
         <v>10.0</v>
       </c>
       <c r="B88" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C88" s="23" t="s">
         <v>9</v>
@@ -4501,27 +4503,27 @@
         <f t="shared" si="8"/>
         <v>August</v>
       </c>
-      <c r="F88" s="30">
+      <c r="F88" s="31">
         <v>100000.0</v>
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="27" t="str">
+      <c r="A89" s="28" t="str">
         <f>E88</f>
         <v>August</v>
       </c>
-      <c r="B89" s="28"/>
-      <c r="C89" s="28"/>
-      <c r="D89" s="28"/>
-      <c r="E89" s="28"/>
-      <c r="F89" s="29"/>
+      <c r="B89" s="29"/>
+      <c r="C89" s="29"/>
+      <c r="D89" s="29"/>
+      <c r="E89" s="29"/>
+      <c r="F89" s="30"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="22">
         <v>1.0</v>
       </c>
       <c r="B90" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C90" s="23" t="s">
         <v>8</v>
@@ -4533,7 +4535,7 @@
         <f t="shared" ref="E90:E99" si="9">TEXT(D90,"MMMM")</f>
         <v>September</v>
       </c>
-      <c r="F90" s="30">
+      <c r="F90" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -4542,7 +4544,7 @@
         <v>2.0</v>
       </c>
       <c r="B91" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C91" s="23" t="s">
         <v>6</v>
@@ -4554,7 +4556,7 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F91" s="30">
+      <c r="F91" s="31">
         <v>450000.0</v>
       </c>
     </row>
@@ -4563,7 +4565,7 @@
         <v>3.0</v>
       </c>
       <c r="B92" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C92" s="23" t="s">
         <v>6</v>
@@ -4575,7 +4577,7 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F92" s="30">
+      <c r="F92" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -4584,7 +4586,7 @@
         <v>4.0</v>
       </c>
       <c r="B93" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C93" s="23" t="s">
         <v>6</v>
@@ -4596,7 +4598,7 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F93" s="30">
+      <c r="F93" s="31">
         <v>150000.0</v>
       </c>
     </row>
@@ -4605,7 +4607,7 @@
         <v>5.0</v>
       </c>
       <c r="B94" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C94" s="23" t="s">
         <v>7</v>
@@ -4617,7 +4619,7 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F94" s="30">
+      <c r="F94" s="31">
         <v>900000.0</v>
       </c>
     </row>
@@ -4638,7 +4640,7 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F95" s="30">
+      <c r="F95" s="31">
         <v>250000.0</v>
       </c>
     </row>
@@ -4647,7 +4649,7 @@
         <v>7.0</v>
       </c>
       <c r="B96" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C96" s="23" t="s">
         <v>5</v>
@@ -4659,7 +4661,7 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F96" s="30">
+      <c r="F96" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -4668,7 +4670,7 @@
         <v>8.0</v>
       </c>
       <c r="B97" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C97" s="23" t="s">
         <v>4</v>
@@ -4680,7 +4682,7 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F97" s="30">
+      <c r="F97" s="31">
         <v>365000.0</v>
       </c>
     </row>
@@ -4701,7 +4703,7 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F98" s="30">
+      <c r="F98" s="31">
         <v>1000000.0</v>
       </c>
     </row>
@@ -4710,7 +4712,7 @@
         <v>10.0</v>
       </c>
       <c r="B99" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C99" s="23" t="s">
         <v>9</v>
@@ -4722,27 +4724,27 @@
         <f t="shared" si="9"/>
         <v>September</v>
       </c>
-      <c r="F99" s="30">
+      <c r="F99" s="31">
         <v>100000.0</v>
       </c>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="27" t="str">
+      <c r="A100" s="28" t="str">
         <f>E99</f>
         <v>September</v>
       </c>
-      <c r="B100" s="28"/>
-      <c r="C100" s="28"/>
-      <c r="D100" s="28"/>
-      <c r="E100" s="28"/>
-      <c r="F100" s="29"/>
+      <c r="B100" s="29"/>
+      <c r="C100" s="29"/>
+      <c r="D100" s="29"/>
+      <c r="E100" s="29"/>
+      <c r="F100" s="30"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="22">
         <v>1.0</v>
       </c>
       <c r="B101" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C101" s="23" t="s">
         <v>8</v>
@@ -4754,7 +4756,7 @@
         <f t="shared" ref="E101:E110" si="10">TEXT(D101,"MMMM")</f>
         <v>October</v>
       </c>
-      <c r="F101" s="30">
+      <c r="F101" s="31">
         <v>1000000.0</v>
       </c>
     </row>
@@ -4763,7 +4765,7 @@
         <v>2.0</v>
       </c>
       <c r="B102" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C102" s="23" t="s">
         <v>6</v>
@@ -4775,7 +4777,7 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F102" s="30">
+      <c r="F102" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -4784,7 +4786,7 @@
         <v>3.0</v>
       </c>
       <c r="B103" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C103" s="23" t="s">
         <v>6</v>
@@ -4796,7 +4798,7 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F103" s="30">
+      <c r="F103" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -4805,7 +4807,7 @@
         <v>4.0</v>
       </c>
       <c r="B104" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C104" s="23" t="s">
         <v>6</v>
@@ -4817,7 +4819,7 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F104" s="30">
+      <c r="F104" s="31">
         <v>365000.0</v>
       </c>
     </row>
@@ -4826,7 +4828,7 @@
         <v>5.0</v>
       </c>
       <c r="B105" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C105" s="23" t="s">
         <v>7</v>
@@ -4838,7 +4840,7 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F105" s="30">
+      <c r="F105" s="31">
         <v>150000.0</v>
       </c>
     </row>
@@ -4859,7 +4861,7 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F106" s="30">
+      <c r="F106" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -4868,7 +4870,7 @@
         <v>7.0</v>
       </c>
       <c r="B107" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C107" s="23" t="s">
         <v>5</v>
@@ -4880,7 +4882,7 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F107" s="30">
+      <c r="F107" s="31">
         <v>900000.0</v>
       </c>
     </row>
@@ -4889,7 +4891,7 @@
         <v>8.0</v>
       </c>
       <c r="B108" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C108" s="23" t="s">
         <v>4</v>
@@ -4901,7 +4903,7 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F108" s="30">
+      <c r="F108" s="31">
         <v>250000.0</v>
       </c>
     </row>
@@ -4922,7 +4924,7 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F109" s="30">
+      <c r="F109" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -4931,7 +4933,7 @@
         <v>10.0</v>
       </c>
       <c r="B110" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C110" s="23" t="s">
         <v>9</v>
@@ -4943,27 +4945,27 @@
         <f t="shared" si="10"/>
         <v>October</v>
       </c>
-      <c r="F110" s="30">
+      <c r="F110" s="31">
         <v>450000.0</v>
       </c>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="27" t="str">
+      <c r="A111" s="28" t="str">
         <f>E110</f>
         <v>October</v>
       </c>
-      <c r="B111" s="28"/>
-      <c r="C111" s="28"/>
-      <c r="D111" s="28"/>
-      <c r="E111" s="28"/>
-      <c r="F111" s="29"/>
+      <c r="B111" s="29"/>
+      <c r="C111" s="29"/>
+      <c r="D111" s="29"/>
+      <c r="E111" s="29"/>
+      <c r="F111" s="30"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="22">
         <v>1.0</v>
       </c>
       <c r="B112" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C112" s="23" t="s">
         <v>8</v>
@@ -4975,7 +4977,7 @@
         <f t="shared" ref="E112:E121" si="11">TEXT(D112,"MMMM")</f>
         <v>November</v>
       </c>
-      <c r="F112" s="30">
+      <c r="F112" s="31">
         <v>900000.0</v>
       </c>
     </row>
@@ -4984,7 +4986,7 @@
         <v>2.0</v>
       </c>
       <c r="B113" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C113" s="23" t="s">
         <v>6</v>
@@ -4996,7 +4998,7 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F113" s="30">
+      <c r="F113" s="31">
         <v>1000000.0</v>
       </c>
     </row>
@@ -5005,7 +5007,7 @@
         <v>3.0</v>
       </c>
       <c r="B114" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C114" s="23" t="s">
         <v>6</v>
@@ -5017,7 +5019,7 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F114" s="30">
+      <c r="F114" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -5026,7 +5028,7 @@
         <v>4.0</v>
       </c>
       <c r="B115" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C115" s="23" t="s">
         <v>6</v>
@@ -5038,7 +5040,7 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F115" s="30">
+      <c r="F115" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -5047,7 +5049,7 @@
         <v>5.0</v>
       </c>
       <c r="B116" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C116" s="23" t="s">
         <v>7</v>
@@ -5059,7 +5061,7 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F116" s="30">
+      <c r="F116" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -5080,7 +5082,7 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F117" s="30">
+      <c r="F117" s="31">
         <v>450000.0</v>
       </c>
     </row>
@@ -5089,7 +5091,7 @@
         <v>7.0</v>
       </c>
       <c r="B118" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C118" s="23" t="s">
         <v>5</v>
@@ -5101,7 +5103,7 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F118" s="30">
+      <c r="F118" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -5110,7 +5112,7 @@
         <v>8.0</v>
       </c>
       <c r="B119" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C119" s="23" t="s">
         <v>4</v>
@@ -5122,7 +5124,7 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F119" s="30">
+      <c r="F119" s="31">
         <v>150000.0</v>
       </c>
     </row>
@@ -5143,7 +5145,7 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F120" s="30">
+      <c r="F120" s="31">
         <v>365000.0</v>
       </c>
     </row>
@@ -5152,7 +5154,7 @@
         <v>10.0</v>
       </c>
       <c r="B121" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C121" s="23" t="s">
         <v>9</v>
@@ -5164,27 +5166,27 @@
         <f t="shared" si="11"/>
         <v>November</v>
       </c>
-      <c r="F121" s="30">
+      <c r="F121" s="31">
         <v>250000.0</v>
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="27" t="str">
+      <c r="A122" s="28" t="str">
         <f>E121</f>
         <v>November</v>
       </c>
-      <c r="B122" s="28"/>
-      <c r="C122" s="28"/>
-      <c r="D122" s="28"/>
-      <c r="E122" s="28"/>
-      <c r="F122" s="29"/>
+      <c r="B122" s="29"/>
+      <c r="C122" s="29"/>
+      <c r="D122" s="29"/>
+      <c r="E122" s="29"/>
+      <c r="F122" s="30"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="22">
         <v>1.0</v>
       </c>
       <c r="B123" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C123" s="23" t="s">
         <v>8</v>
@@ -5196,7 +5198,7 @@
         <f t="shared" ref="E123:E132" si="12">TEXT(D123,"MMMM")</f>
         <v>December</v>
       </c>
-      <c r="F123" s="30">
+      <c r="F123" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -5205,7 +5207,7 @@
         <v>2.0</v>
       </c>
       <c r="B124" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C124" s="23" t="s">
         <v>6</v>
@@ -5217,7 +5219,7 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F124" s="30">
+      <c r="F124" s="31">
         <v>900000.0</v>
       </c>
     </row>
@@ -5226,7 +5228,7 @@
         <v>3.0</v>
       </c>
       <c r="B125" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C125" s="23" t="s">
         <v>6</v>
@@ -5238,7 +5240,7 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F125" s="30">
+      <c r="F125" s="31">
         <v>150000.0</v>
       </c>
     </row>
@@ -5247,7 +5249,7 @@
         <v>4.0</v>
       </c>
       <c r="B126" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C126" s="23" t="s">
         <v>6</v>
@@ -5259,7 +5261,7 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F126" s="30">
+      <c r="F126" s="31">
         <v>450000.0</v>
       </c>
     </row>
@@ -5268,7 +5270,7 @@
         <v>5.0</v>
       </c>
       <c r="B127" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C127" s="23" t="s">
         <v>7</v>
@@ -5280,7 +5282,7 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F127" s="30">
+      <c r="F127" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -5301,7 +5303,7 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F128" s="30">
+      <c r="F128" s="31">
         <v>365000.0</v>
       </c>
     </row>
@@ -5310,7 +5312,7 @@
         <v>7.0</v>
       </c>
       <c r="B129" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C129" s="23" t="s">
         <v>5</v>
@@ -5322,7 +5324,7 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F129" s="30">
+      <c r="F129" s="31">
         <v>1000000.0</v>
       </c>
     </row>
@@ -5331,7 +5333,7 @@
         <v>8.0</v>
       </c>
       <c r="B130" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C130" s="23" t="s">
         <v>4</v>
@@ -5343,7 +5345,7 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F130" s="30">
+      <c r="F130" s="31">
         <v>250000.0</v>
       </c>
     </row>
@@ -5364,7 +5366,7 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F131" s="30">
+      <c r="F131" s="31">
         <v>100000.0</v>
       </c>
     </row>
@@ -5373,7 +5375,7 @@
         <v>10.0</v>
       </c>
       <c r="B132" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C132" s="23" t="s">
         <v>9</v>
@@ -5385,20 +5387,20 @@
         <f t="shared" si="12"/>
         <v>December</v>
       </c>
-      <c r="F132" s="30">
+      <c r="F132" s="31">
         <v>100000.0</v>
       </c>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="27" t="str">
+      <c r="A133" s="28" t="str">
         <f>E132</f>
         <v>December</v>
       </c>
-      <c r="B133" s="28"/>
-      <c r="C133" s="28"/>
-      <c r="D133" s="28"/>
-      <c r="E133" s="28"/>
-      <c r="F133" s="29"/>
+      <c r="B133" s="29"/>
+      <c r="C133" s="29"/>
+      <c r="D133" s="29"/>
+      <c r="E133" s="29"/>
+      <c r="F133" s="30"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
       <c r="C134" s="23"/>

</xml_diff>